<commit_message>
single ver: update get value from excel
</commit_message>
<xml_diff>
--- a/DesktopApp/bin/Release/file/ExportExcelCSR.Dialog.xlsx
+++ b/DesktopApp/bin/Release/file/ExportExcelCSR.Dialog.xlsx
@@ -37,26 +37,97 @@
 MIICtDCCAZwCAQAwcTEVMBMGA1UEAwwMTmd1eWVuIFZhbiBCMRQwEgYDVQQLDAtD
 b25nIFR5IEFCQzEUMBIGA1UECgwLQ29uZyBUeSBBQkMxCzAJBgNVBAYTAlZOMQ8w
 DQYDVQQHDAZRdWFuIDExDjAMBgNVBAgMBVRQSENNMIIBIjANBgkqhkiG9w0BAQEF
-AAOCAQ8AMIIBCgKCAQEAvy/Thl6+6qGCHZrZeyF/nljNv8qTyN5BIQKMusZr9MZQ
-+eRFk9OuoulBHQ2UgtpKIwlO70LEIq9pvtnWptB0Zcto6xMh+JqxhZx35zwoZswR
-A6bIjXcpO3ndShJLYMtbJS0LbdPg4nnwq0pYQWWXuvSJYVExIxRpyE4hEF5BrUbH
-0NIS3dCKQVvK8BCe3pdrPrhKKe+zWJDQCIN/p8GHeAQEk25Y4V+2qJx2Uqmcx3ZX
-idZAEPTzMkSR89UsFUCILHBU7vG1uH8ye74f5WnKHHjV84CI5z+uK8Lkd12Sj8Dw
-ILF2KJOomQS1PdAV2ZssD1TH/B03akYTg48hcFyDtQIDAQABMA0GCSqGSIb3DQEB
-BQUAA4IBAQAreJ9jXBvpHpIiGCV+7O8Rsvqjvbaw4vrXY4T4C1JAwjvol53kPTND
-L1MY0M///eO+vHcidxknRsIEOgxcMZB3rgldKZ+FeLUqXGG0LOhXs8wVX1E3Bv1g
-FTtiHZXRe5mYsLN6kFED7rQbZedW18I9yFqW/w/7BRR4TzRqW+QSuCiO+fOQjJpP
-1BAolZ5gJ+GwzylSXiOEXN8ozucNOx7Hjjo9fYw4E6gYPUqk/wJ4X7tbUOnoruTN
-sJ/ncL0NbMPewoErEJ88+VSDXjlxdz56ji+82z+SYezszCoWg0gVADYM2QiIaPzT
-TfEXU6pUD3fu1O+jjjYKmFiwcj8ohrFt
+AAOCAQ8AMIIBCgKCAQEAkz8TL4dqCIiJ7KnHFBAFe82+5HPYo5xfk1LataHfu4Uj
+xOxCBv6M3F45NHenwi2VZlaclnW2yWU+TitWMTmbWxs5x0JJqxmHzHDclSOAp8Mv
+uTxSR0cxv5OSYoagoiwNE0OcjlYSg3lWISnyGsskYGLa9+GXBE4nquVgS23AiKxH
+5EDEWEBPFraYXFl51OXUm2oztPUMgbhDJRcg2bVZfJrzgFHIcvt8x6UMwYbsSO0U
+bJDXTUyT96BMlAm70g0piu8V6h0firLaD6/+7HKFCMYWYe4q1DbmWGiVxUeZ8cHg
+3iX8xYw1+xCgCFTbsMjBw4ijpApRHg650V9aVecaYwIDAQABMA0GCSqGSIb3DQEB
+BQUAA4IBAQBj9LixX5puB3DPKQsi5EaalujLGnPVWekvAJw/24F3jOABa+r7y1ou
+1BCcgIeopG2NdGJheM3YGD6XzIPjNSVWSeBhGri+QPsRo4I3KFM/waqLQVzE5tZv
+U9sbGVcq4F5iYEV5AWkgXyOr3GBDExsbeej8WsS1cYBOpNMwKBJv/JAhPny7nkkr
+7j51qsZsT/G33UPxXayG6uiAxAUT6IzlKRJfV9hETOauc2m71ybrd3pzbtGBlWIN
+mvESBrGtg6UWbbGboIpCwUIXOIDMORKWnSdBy9itbs8etx8I57YYaqDHV/bD3baQ
+qG7gpHrUvRnuzAAe2PRJ71VElqCyAYLU
 -----END CERTIFICATE REQUEST-----
 </t>
   </si>
   <si>
-    <t>MIIGZzCCBE+gAwIBAgIMJcSn9Jru5Q1JkgBAMA0GCSqGSIb3DQEBCwUAMIHIMQswCQYDVQQGEwJWTjEUMBIGA1UECBMLSG8gQ2hpIE1pbmgxFDASBgNVBAcTC0hvIENoaSBNaW5oMUAwPgYDVQQKEzdNb2JpbGUtSUQgVGVjaG5vbG9naWVzIGFuZCBTZXJ2aWNlcyBKb2ludCBTdG9jayBDb21wYW55MScwJQYDVQQLEx5Nb2JpbGUtSUQgVGVjaG5pY2FsIERlcGFydG1lbnQxIjAgBgNVBAMTGU1vYmlsZS1JRCBUcnVzdGVkIE5ldHdvcmswHhcNMjIwODA4MDE1MTEyWhcNMjMwODEzMDE1MTEyWjCBlDELMAkGA1UEBhMCVk4xEzARBgNVBAgMCkPhuqduIFRoxqExGjAYBgNVBAoMEU5ndXllbiBWYW4gVGVzdCAyMRcwFQYDVQQLDA5Db25nIFR5IEFCQ0QgMjEaMBgGA1UEAwwRTmd1eWVuIFZhbiBUZXN0IDIxHzAdBgoJkiaJk/IsZAEBDA9NU1Q6MTIzNDU2NzgwMDUwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQC/L9OGXr7qoYIdmtl7IX+eWM2/ypPI3kEhAoy6xmv0xlD55EWT066i6UEdDZSC2kojCU7vQsQir2m+2dam0HRly2jrEyH4mrGFnHfnPChmzBEDpsiNdyk7ed1KEktgy1slLQtt0+DiefCrSlhBZZe69IlhUTEjFGnITiEQXkGtRsfQ0hLd0IpBW8rwEJ7el2s+uEop77NYkNAIg3+nwYd4BASTbljhX7aonHZSqZzHdleJ1kAQ9PMyRJHz1SwVQIgscFTu8bW4fzJ7vh/lacoceNXzgIjnP64rwuR3XZKPwPAgsXYok6iZBLU90BXZmywPVMf8HTdqRhODjyFwXIO1AgMBAAGjggGBMIIBfTAMBgNVHRMBAf8EAjAAMB8GA1UdIwQYMBaAFPNkMn2yPF3lLuBJfLTqYhWUeC6rMHIGCCsGAQUFBwEBBGYwZDAyBggrBgEFBQcwAoYmaHR0cHM6Ly9tb2JpbGUtaWQudm4vcGtpL21vYmlsZS1pZC5jcnQwLgYIKwYBBQUHMAGGImh0dHA6Ly9tb2JpbGUtaWQudm4vb2NzcC9yZXNwb25kZXIwRQYDVR0gBD4wPDA6BgsrBgEEAYHtAwEEATArMCkGCCsGAQUFBwIBFh1odHRwczovL21vYmlsZS1pZC52bi9jcHMuaHRtbDA0BgNVHSUELTArBggrBgEFBQcDAgYIKwYBBQUHAwQGCisGAQQBgjcKAwwGCSqGSIb3LwEBBTAsBgNVHR8EJTAjMCGgH6AdhhtodHRwOi8vbW9iaWxlLWlkLnZuL2NybC9nZXQwHQYDVR0OBBYEFNe71pRVjX8AejArwTVdZgYfUjCSMA4GA1UdDwEB/wQEAwIE8DANBgkqhkiG9w0BAQsFAAOCAgEAVQTzptjr+GH7Yav1VAK7DEiklPamC1QJQQfrTu3AZxcbD9H1lHMCGdhrJcX4AJFMyaGrsQvfYEAwpWpfk9h2mUmFsTSyrvMU3xUeIs+wMSibQwhALM97yc0dmCt8YcMzVreITeCismFidJq62RVB4CwPoWpAkRC8Iup3pv6B5nASKFe3MVpBYELD+/dXOh66x5vaWdo3GAn1XEXMc16PZqhtHlThgabq94WQwosV9dE4bcGlY2dJl22D4zg4NmytTO04pBSqLEz3dCEbZbn9gcCM+8oGX4XjuRFp4To2r9aYOcYfZsQL6JJya3Erv3jaTc0x1ouhxrMTS9qjQvoOMsLCUnOXjAt96mUYdHPfETb0lJki9XNn2vlmqIuKzI2y0ZmQcJWyh5jiKIyFLhEU+vCvSoijLw+AKFgONG9wbnenOkr3VLrI7ZzeEUtGAtI8Vyu3XJEivKOLh330qGrNfsm+xbrXQZjtZ/I2RUaWAndVg8LeGt8RlQQ3g7IVEripxKQn0z7rhIRHqcTa/o0nZXYdxvS6tqyvEOFz0CkReOEbIr8bQyHhtPDErakQOLrYHrW9h64LoLygI2qhzD7VfAFujlfgg+9f/UIylcAOLO8kX4JhbXNxdW1NSdDwdQLxqxw5hSRNbNN792wgw3QTApFTOhQlfvuGyA1MZ6B6UQE=</t>
-  </si>
-  <si>
-    <t>MIIGRDCCBCygAwIBAgIEVfAPITANBgkqhkiG9w0BAQsFADCByDELMAkGA1UEBhMCVk4xFDASBgNVBAgTC0hvIENoaSBNaW5oMRQwEgYDVQQHEwtIbyBDaGkgTWluaDFAMD4GA1UEChM3TW9iaWxlLUlEIFRlY2hub2xvZ2llcyBhbmQgU2VydmljZXMgSm9pbnQgU3RvY2sgQ29tcGFueTEnMCUGA1UECxMeTW9iaWxlLUlEIFRlY2huaWNhbCBEZXBhcnRtZW50MSIwIAYDVQQDExlNb2JpbGUtSUQgVHJ1c3RlZCBOZXR3b3JrMCAXDTE3MDQyMTAyNTA1MVoYDzIxMTcwMzI4MDI1MDUxWjCByDELMAkGA1UEBhMCVk4xFDASBgNVBAgTC0hvIENoaSBNaW5oMRQwEgYDVQQHEwtIbyBDaGkgTWluaDFAMD4GA1UEChM3TW9iaWxlLUlEIFRlY2hub2xvZ2llcyBhbmQgU2VydmljZXMgSm9pbnQgU3RvY2sgQ29tcGFueTEnMCUGA1UECxMeTW9iaWxlLUlEIFRlY2huaWNhbCBEZXBhcnRtZW50MSIwIAYDVQQDExlNb2JpbGUtSUQgVHJ1c3RlZCBOZXR3b3JrMIICIjANBgkqhkiG9w0BAQEFAAOCAg8AMIICCgKCAgEAjtHJbKRUfVPE3vr7SjROLgQYO1bTi+WgIinSsLn9XGj7gjO4cx8ejs9I8IGrx2q5Wzcrcavi5nxRzoKbO8EVkR+F69UxgF54e8Nfe76i3v8BGTk8vngpvQrndN8uE6YiQ/G0s5hLi/gZfffcMTlMQrlwYdRpEMhn6nNoF675xpaBk15+epa7SjXbgGvCkA0CkR+SKvhd4pnMORZ2/jpQvLG5DQIzQLApAmWHcoexFxTgPzuw2qhinWPO07X/H5pz5dAAKhflI451OG2PZCloZEo1lemmspm3azFlaYzkbLPI+GsV61PB/AQEIKq9tXLCuyYbpXYqOlbFP8LYGyfumdOwS2/LFKwHGLAdlofCGI0eMp/dsa+aL+My8Rqv0S0PhClcnvDaSCIYBPDgI5wW4u/sr3Wz5n5f4Z3k5vJi0GU8l0FroNsFCN8EOc/vM+wgm+Uol74FrEo0LpT8TUWh71HUF29sBxtEQ8Zw5YpUMCTcPuBsVRwuLGGae8VKpPc4jEwpGmvoGj8cfS2qoEMNPtRnGM3Kt+q39zLoDk+6Kmr5oi8XVfZmibXRtNvrixMj6jAEm/3Vag9VdQ4SR+QFwpJOcIOBtX9mDnamXnBHWFqGUqOUU9/6y4p8B2o3RDE/WeiWtU66gQZasli6TJb0RpNoY/XyXHGn+J0gd9EDXn0CAwEAAaMyMDAwDwYDVR0TAQH/BAUwAwEB/zAdBgNVHQ4EFgQU82QyfbI8XeUu4El8tOpiFZR4LqswDQYJKoZIhvcNAQELBQADggIBAI3hBTzed1ZtDh5DvdidSJoGRBXJQ24Y3VjxPbelLNxnZiYCiSIQhL7KIjmDZOBQJwqlBxWOsao7PuRaohdAcDQ2jImeiIAmkRaTcUWZgB++IuS1ta01XMcAEp/taQEjHKjwAr22IILNVk9z0WNVf5Pd9NWMu4lFqwECpKTJnToIqEGVVWcqAAupGT64LQ/Cf+/oEpDtkRaVazFj7ob1Rxjl5hmOxMwNHW8wRPcq8glg+26Tp9jqcaw32fhfnUPDHBdoYcU/VhMkgBeYXGHTPHp32Kj4l/QxWnxY0IvChyq+Qao1D19K5PbJQH5A5bQbwqgBtMihsdrGSr9VJ7LtNmBc+8dNchqi2uXs3ryk8htDluZ60yWK89eRO1NatB2tiDLh5iwejJRieOoyQ3Iq8m/IjtEJTs7ehWJHtiGj2U/tlpVW2fSszoz0TbKxXQPQ/dGNmDorqrM/0WEY6lkNEp7qbXB1U378PFUKFh1lIdlfNrgoEvYt0XeIMbXn+fUkB8munP0bCSiJqX7gK+2FuZqfA038JfuwxDBr8SvkkvZOqyUgMPAPRpQCjmFrZgMrilHUokZIL5+Cz4qaxEf3s3xORy+CuPMousfrOKpdf6jFjnyD8cr4Ez4bMAekPg4F4JJ0WHpOchSlDP5a57cb6mHYvOF8ygSobADyNeQ1jkjg</t>
+    <t>"-----BEGIN CERTIFICATE-----
+MIIGZDCCBEygAwIBAgIMPRw66sJFvKK12gGJMA0GCSqGSIb3DQEBCwUAMIHIMQsw
+CQYDVQQGEwJWTjEUMBIGA1UECBMLSG8gQ2hpIE1pbmgxFDASBgNVBAcTC0hvIENo
+aSBNaW5oMUAwPgYDVQQKEzdNb2JpbGUtSUQgVGVjaG5vbG9naWVzIGFuZCBTZXJ2
+aWNlcyBKb2ludCBTdG9jayBDb21wYW55MScwJQYDVQQLEx5Nb2JpbGUtSUQgVGVj
+aG5pY2FsIERlcGFydG1lbnQxIjAgBgNVBAMTGU1vYmlsZS1JRCBUcnVzdGVkIE5l
+dHdvcmswHhcNMjIwODA4MDc0OTQ2WhcNMjMwODEzMDc0OTQ2WjCBkTELMAkGA1UE
+BhMCVk4xEjAQBgNVBAgMCUjDoCBO4buZaTEaMBgGA1UECgwRTmd1eWVuIFZhbiBU
+ZXN0IDgxFTATBgNVBAsMDENvbmcgVHkgQUJDRDEaMBgGA1UEAwwRTmd1eWVuIFZh
+biBUZXN0IDgxHzAdBgoJkiaJk/IsZAEBDA9NU1Q6MTIzNDU2NzgwMDgwggEiMA0G
+CSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCTPxMvh2oIiInsqccUEAV7zb7kc9ij
+nF+TUtq1od+7hSPE7EIG/ozcXjk0d6fCLZVmVpyWdbbJZT5OK1YxOZtbGznHQkmr
+GYfMcNyVI4Cnwy+5PFJHRzG/k5JihqCiLA0TQ5yOVhKDeVYhKfIayyRgYtr34ZcE
+Tieq5WBLbcCIrEfkQMRYQE8WtphcWXnU5dSbajO09QyBuEMlFyDZtVl8mvOAUchy
++3zHpQzBhuxI7RRskNdNTJP3oEyUCbvSDSmK7xXqHR+KstoPr/7scoUIxhZh7irU
+NuZYaJXFR5nxweDeJfzFjDX7EKAIVNuwyMHDiKOkClEeDrnRX1pV5xpjAgMBAAGj
+ggGBMIIBfTAMBgNVHRMBAf8EAjAAMB8GA1UdIwQYMBaAFPNkMn2yPF3lLuBJfLTq
+YhWUeC6rMHIGCCsGAQUFBwEBBGYwZDAyBggrBgEFBQcwAoYmaHR0cHM6Ly9tb2Jp
+bGUtaWQudm4vcGtpL21vYmlsZS1pZC5jcnQwLgYIKwYBBQUHMAGGImh0dHA6Ly9t
+b2JpbGUtaWQudm4vb2NzcC9yZXNwb25kZXIwRQYDVR0gBD4wPDA6BgsrBgEEAYHt
+AwEEATArMCkGCCsGAQUFBwIBFh1odHRwczovL21vYmlsZS1pZC52bi9jcHMuaHRt
+bDA0BgNVHSUELTArBggrBgEFBQcDAgYIKwYBBQUHAwQGCisGAQQBgjcKAwwGCSqG
+SIb3LwEBBTAsBgNVHR8EJTAjMCGgH6AdhhtodHRwOi8vbW9iaWxlLWlkLnZuL2Ny
+bC9nZXQwHQYDVR0OBBYEFO6StLdmB5DjmNjninoUuSL3aAzrMA4GA1UdDwEB/wQE
+AwIE8DANBgkqhkiG9w0BAQsFAAOCAgEALYDRvZ6f4dWlUClnZnngT3CuVExFW8iZ
+zTN4T3G7mXU5CqzgXjW36QFY7TIXBVxjqNYhgB1gIe85AjZhjrnAWuuKRVMrpgde
+P/ZiuQ6ZTiQzUi1EuOPJhp6j8tUPjbzS+oBx9xFTAL2XUez6Xqv6wly/EWs6ca7B
+v3YiKksgC2HbLIIKXKcJMxCbMK26uzhfj8J3jL+ioQfCu+MiaTAu0pJblA/5gyIz
+fYnKD9On0at5m2QTYNoPyoi+DtlK/AQb+hziEnnsq0g2kG6yfiREB4M4EsbvRYMm
+FjoDVSIipnWr3wvwOmBlo9YEMTTtXHPNR5cGHZn6spBRUXir8NdRlz0CFxsUzd+i
+9whZPnUORyprDZEmFVleNvkvs3kk7sdbNmInlLFdY9bsVx0AM80Bq2KSjuC7kWat
+8d5LLhUIc00p+IRHQPAri9Bb1aX1AVBcAyqhUvahz4qiM8/lrWDepYAeqJeFtHzS
+4NfZHJGxQqK0qycj0WzzRCdzmDjKDTCLfMCU0Bp++tbthD42BlPfr1ifgBZ2y54M
+dKxSEJMyKAA5KCzadRLnaTA427ei4tvw599yvcxvYGoyRVvLzi/eqWD3o8ENKKbe
+l+z8l+3C2ZwYWm1hAn3AVzHb4n1dfuUpEQ82syfuqCcLAFYhPMSIBMsrteeYgddM
+XNtg/VC+tDI=
+-----END CERTIFICATE-----"</t>
+  </si>
+  <si>
+    <t>"-----BEGIN CERTIFICATE-----
+MIIGRDCCBCygAwIBAgIEVfAPITANBgkqhkiG9w0BAQsFADCByDELMAkGA1UEBhMC
+Vk4xFDASBgNVBAgTC0hvIENoaSBNaW5oMRQwEgYDVQQHEwtIbyBDaGkgTWluaDFA
+MD4GA1UEChM3TW9iaWxlLUlEIFRlY2hub2xvZ2llcyBhbmQgU2VydmljZXMgSm9p
+bnQgU3RvY2sgQ29tcGFueTEnMCUGA1UECxMeTW9iaWxlLUlEIFRlY2huaWNhbCBE
+ZXBhcnRtZW50MSIwIAYDVQQDExlNb2JpbGUtSUQgVHJ1c3RlZCBOZXR3b3JrMCAX
+DTE3MDQyMTAyNTA1MVoYDzIxMTcwMzI4MDI1MDUxWjCByDELMAkGA1UEBhMCVk4x
+FDASBgNVBAgTC0hvIENoaSBNaW5oMRQwEgYDVQQHEwtIbyBDaGkgTWluaDFAMD4G
+A1UEChM3TW9iaWxlLUlEIFRlY2hub2xvZ2llcyBhbmQgU2VydmljZXMgSm9pbnQg
+U3RvY2sgQ29tcGFueTEnMCUGA1UECxMeTW9iaWxlLUlEIFRlY2huaWNhbCBEZXBh
+cnRtZW50MSIwIAYDVQQDExlNb2JpbGUtSUQgVHJ1c3RlZCBOZXR3b3JrMIICIjAN
+BgkqhkiG9w0BAQEFAAOCAg8AMIICCgKCAgEAjtHJbKRUfVPE3vr7SjROLgQYO1bT
+i+WgIinSsLn9XGj7gjO4cx8ejs9I8IGrx2q5Wzcrcavi5nxRzoKbO8EVkR+F69Ux
+gF54e8Nfe76i3v8BGTk8vngpvQrndN8uE6YiQ/G0s5hLi/gZfffcMTlMQrlwYdRp
+EMhn6nNoF675xpaBk15+epa7SjXbgGvCkA0CkR+SKvhd4pnMORZ2/jpQvLG5DQIz
+QLApAmWHcoexFxTgPzuw2qhinWPO07X/H5pz5dAAKhflI451OG2PZCloZEo1lemm
+spm3azFlaYzkbLPI+GsV61PB/AQEIKq9tXLCuyYbpXYqOlbFP8LYGyfumdOwS2/L
+FKwHGLAdlofCGI0eMp/dsa+aL+My8Rqv0S0PhClcnvDaSCIYBPDgI5wW4u/sr3Wz
+5n5f4Z3k5vJi0GU8l0FroNsFCN8EOc/vM+wgm+Uol74FrEo0LpT8TUWh71HUF29s
+BxtEQ8Zw5YpUMCTcPuBsVRwuLGGae8VKpPc4jEwpGmvoGj8cfS2qoEMNPtRnGM3K
+t+q39zLoDk+6Kmr5oi8XVfZmibXRtNvrixMj6jAEm/3Vag9VdQ4SR+QFwpJOcIOB
+tX9mDnamXnBHWFqGUqOUU9/6y4p8B2o3RDE/WeiWtU66gQZasli6TJb0RpNoY/Xy
+XHGn+J0gd9EDXn0CAwEAAaMyMDAwDwYDVR0TAQH/BAUwAwEB/zAdBgNVHQ4EFgQU
+82QyfbI8XeUu4El8tOpiFZR4LqswDQYJKoZIhvcNAQELBQADggIBAI3hBTzed1Zt
+Dh5DvdidSJoGRBXJQ24Y3VjxPbelLNxnZiYCiSIQhL7KIjmDZOBQJwqlBxWOsao7
+PuRaohdAcDQ2jImeiIAmkRaTcUWZgB++IuS1ta01XMcAEp/taQEjHKjwAr22IILN
+Vk9z0WNVf5Pd9NWMu4lFqwECpKTJnToIqEGVVWcqAAupGT64LQ/Cf+/oEpDtkRaV
+azFj7ob1Rxjl5hmOxMwNHW8wRPcq8glg+26Tp9jqcaw32fhfnUPDHBdoYcU/VhMk
+gBeYXGHTPHp32Kj4l/QxWnxY0IvChyq+Qao1D19K5PbJQH5A5bQbwqgBtMihsdrG
+Sr9VJ7LtNmBc+8dNchqi2uXs3ryk8htDluZ60yWK89eRO1NatB2tiDLh5iwejJRi
+eOoyQ3Iq8m/IjtEJTs7ehWJHtiGj2U/tlpVW2fSszoz0TbKxXQPQ/dGNmDorqrM/
+0WEY6lkNEp7qbXB1U378PFUKFh1lIdlfNrgoEvYt0XeIMbXn+fUkB8munP0bCSiJ
+qX7gK+2FuZqfA038JfuwxDBr8SvkkvZOqyUgMPAPRpQCjmFrZgMrilHUokZIL5+C
+z4qaxEf3s3xORy+CuPMousfrOKpdf6jFjnyD8cr4Ez4bMAekPg4F4JJ0WHpOchSl
+DP5a57cb6mHYvOF8ygSobADyNeQ1jkjg
+-----END CERTIFICATE-----"</t>
   </si>
 </sst>
 </file>
@@ -92,8 +163,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,7 +451,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,17 +474,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
single ver: update final
</commit_message>
<xml_diff>
--- a/DesktopApp/bin/Release/file/ExportExcelCSR.Dialog.xlsx
+++ b/DesktopApp/bin/Release/file/ExportExcelCSR.Dialog.xlsx
@@ -37,38 +37,38 @@
 MIICtDCCAZwCAQAwcTEVMBMGA1UEAwwMTmd1eWVuIFZhbiBCMRQwEgYDVQQLDAtD
 b25nIFR5IEFCQzEUMBIGA1UECgwLQ29uZyBUeSBBQkMxCzAJBgNVBAYTAlZOMQ8w
 DQYDVQQHDAZRdWFuIDExDjAMBgNVBAgMBVRQSENNMIIBIjANBgkqhkiG9w0BAQEF
-AAOCAQ8AMIIBCgKCAQEAkz8TL4dqCIiJ7KnHFBAFe82+5HPYo5xfk1LataHfu4Uj
-xOxCBv6M3F45NHenwi2VZlaclnW2yWU+TitWMTmbWxs5x0JJqxmHzHDclSOAp8Mv
-uTxSR0cxv5OSYoagoiwNE0OcjlYSg3lWISnyGsskYGLa9+GXBE4nquVgS23AiKxH
-5EDEWEBPFraYXFl51OXUm2oztPUMgbhDJRcg2bVZfJrzgFHIcvt8x6UMwYbsSO0U
-bJDXTUyT96BMlAm70g0piu8V6h0firLaD6/+7HKFCMYWYe4q1DbmWGiVxUeZ8cHg
-3iX8xYw1+xCgCFTbsMjBw4ijpApRHg650V9aVecaYwIDAQABMA0GCSqGSIb3DQEB
-BQUAA4IBAQBj9LixX5puB3DPKQsi5EaalujLGnPVWekvAJw/24F3jOABa+r7y1ou
-1BCcgIeopG2NdGJheM3YGD6XzIPjNSVWSeBhGri+QPsRo4I3KFM/waqLQVzE5tZv
-U9sbGVcq4F5iYEV5AWkgXyOr3GBDExsbeej8WsS1cYBOpNMwKBJv/JAhPny7nkkr
-7j51qsZsT/G33UPxXayG6uiAxAUT6IzlKRJfV9hETOauc2m71ybrd3pzbtGBlWIN
-mvESBrGtg6UWbbGboIpCwUIXOIDMORKWnSdBy9itbs8etx8I57YYaqDHV/bD3baQ
-qG7gpHrUvRnuzAAe2PRJ71VElqCyAYLU
+AAOCAQ8AMIIBCgKCAQEAhii3SsTFy6g/zPQpufFMbpt33NHlshemGxGdYMfwmUrH
+F5WQ85Y7yhBllZfyRo6IuR+f3QVAhmACynd5QZ2pWZr7wGuFAwfuNo/egO9ctpkX
+gnggOgW/n0lojVThMp/itcSRM9SVwyBvffPmG2CVawXFeV3G+cph5I509cyqxOyf
+oKuwQ48da4YMYFIi+zGgeo2ilBrxL6zPK50Npmstg6MfHNvS98nOgH1PeBgo1OU7
+HP8TVvDh+PfZV8AQQsY/9eGNMCBwoxiphPPj4v+dVqjwihP7UBr13+umnca0no0q
+bwYBGRqtiWVcFYcndWTen/cPppflOfO2wsqgebz+GwIDAQABMA0GCSqGSIb3DQEB
+BQUAA4IBAQBDjEhqfacS34Ec/C9eR7IpNljRQz6WRqPoTq03tQf4RJ9mKq+X5ku8
+rd50XKvb82Lf7uiOiRHwNRzn/yTkOk8n5nl28kanNDbZf4ZVYR+bIYiBXTLumWN+
+9hlmnLuO9bxHo0h1mn0WATvd0ReBE2CkGC6v2+k8Fwv44GBNUa8X+ymc/GsSyV+2
+tdsNh671RsgR0RmIyTdaWWqkU4V/XZlQCOxhX6CPWuXXbMXPZ01XRsv+zls8uk3q
+jkexOoUmZWN2+X7XwuWkhfti/fDG+I7fEG77sT0y7MEKULvmPuS+BaEUs21GGs+W
+1s83sHwB3pzwoSww9yCZ/177PmhU7Cyy
 -----END CERTIFICATE REQUEST-----
 </t>
   </si>
   <si>
     <t>"-----BEGIN CERTIFICATE-----
-MIIGZDCCBEygAwIBAgIMPRw66sJFvKK12gGJMA0GCSqGSIb3DQEBCwUAMIHIMQsw
+MIIGZDCCBEygAwIBAgIMXUQx+s7YNyZcrOJQMA0GCSqGSIb3DQEBCwUAMIHIMQsw
 CQYDVQQGEwJWTjEUMBIGA1UECBMLSG8gQ2hpIE1pbmgxFDASBgNVBAcTC0hvIENo
 aSBNaW5oMUAwPgYDVQQKEzdNb2JpbGUtSUQgVGVjaG5vbG9naWVzIGFuZCBTZXJ2
 aWNlcyBKb2ludCBTdG9jayBDb21wYW55MScwJQYDVQQLEx5Nb2JpbGUtSUQgVGVj
 aG5pY2FsIERlcGFydG1lbnQxIjAgBgNVBAMTGU1vYmlsZS1JRCBUcnVzdGVkIE5l
-dHdvcmswHhcNMjIwODA4MDc0OTQ2WhcNMjMwODEzMDc0OTQ2WjCBkTELMAkGA1UE
+dHdvcmswHhcNMjIwODA4MDkyMjU2WhcNMjMwODEzMDkyMjU2WjCBkTELMAkGA1UE
 BhMCVk4xEjAQBgNVBAgMCUjDoCBO4buZaTEaMBgGA1UECgwRTmd1eWVuIFZhbiBU
-ZXN0IDgxFTATBgNVBAsMDENvbmcgVHkgQUJDRDEaMBgGA1UEAwwRTmd1eWVuIFZh
-biBUZXN0IDgxHzAdBgoJkiaJk/IsZAEBDA9NU1Q6MTIzNDU2NzgwMDgwggEiMA0G
-CSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCTPxMvh2oIiInsqccUEAV7zb7kc9ij
-nF+TUtq1od+7hSPE7EIG/ozcXjk0d6fCLZVmVpyWdbbJZT5OK1YxOZtbGznHQkmr
-GYfMcNyVI4Cnwy+5PFJHRzG/k5JihqCiLA0TQ5yOVhKDeVYhKfIayyRgYtr34ZcE
-Tieq5WBLbcCIrEfkQMRYQE8WtphcWXnU5dSbajO09QyBuEMlFyDZtVl8mvOAUchy
-+3zHpQzBhuxI7RRskNdNTJP3oEyUCbvSDSmK7xXqHR+KstoPr/7scoUIxhZh7irU
-NuZYaJXFR5nxweDeJfzFjDX7EKAIVNuwyMHDiKOkClEeDrnRX1pV5xpjAgMBAAGj
+ZXN0IDkxFTATBgNVBAsMDENvbmcgVHkgQUJDRDEaMBgGA1UEAwwRTmd1eWVuIFZh
+biBUZXN0IDkxHzAdBgoJkiaJk/IsZAEBDA9NU1Q6MTIzNDU2NzgwMDkwggEiMA0G
+CSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCGKLdKxMXLqD/M9Cm58Uxum3fc0eWy
+F6YbEZ1gx/CZSscXlZDzljvKEGWVl/JGjoi5H5/dBUCGYALKd3lBnalZmvvAa4UD
+B+42j96A71y2mReCeCA6Bb+fSWiNVOEyn+K1xJEz1JXDIG998+YbYJVrBcV5Xcb5
+ymHkjnT1zKrE7J+gq7BDjx1rhgxgUiL7MaB6jaKUGvEvrM8rnQ2may2Dox8c29L3
+yc6AfU94GCjU5Tsc/xNW8OH499lXwBBCxj/14Y0wIHCjGKmE8+Pi/51WqPCKE/tQ
+GvXf66adxrSejSpvBgEZGq2JZVwVhyd1ZN6f9w+ml+U587bCyqB5vP4bAgMBAAGj
 ggGBMIIBfTAMBgNVHRMBAf8EAjAAMB8GA1UdIwQYMBaAFPNkMn2yPF3lLuBJfLTq
 YhWUeC6rMHIGCCsGAQUFBwEBBGYwZDAyBggrBgEFBQcwAoYmaHR0cHM6Ly9tb2Jp
 bGUtaWQudm4vcGtpL21vYmlsZS1pZC5jcnQwLgYIKwYBBQUHMAGGImh0dHA6Ly9t
@@ -76,19 +76,19 @@
 AwEEATArMCkGCCsGAQUFBwIBFh1odHRwczovL21vYmlsZS1pZC52bi9jcHMuaHRt
 bDA0BgNVHSUELTArBggrBgEFBQcDAgYIKwYBBQUHAwQGCisGAQQBgjcKAwwGCSqG
 SIb3LwEBBTAsBgNVHR8EJTAjMCGgH6AdhhtodHRwOi8vbW9iaWxlLWlkLnZuL2Ny
-bC9nZXQwHQYDVR0OBBYEFO6StLdmB5DjmNjninoUuSL3aAzrMA4GA1UdDwEB/wQE
-AwIE8DANBgkqhkiG9w0BAQsFAAOCAgEALYDRvZ6f4dWlUClnZnngT3CuVExFW8iZ
-zTN4T3G7mXU5CqzgXjW36QFY7TIXBVxjqNYhgB1gIe85AjZhjrnAWuuKRVMrpgde
-P/ZiuQ6ZTiQzUi1EuOPJhp6j8tUPjbzS+oBx9xFTAL2XUez6Xqv6wly/EWs6ca7B
-v3YiKksgC2HbLIIKXKcJMxCbMK26uzhfj8J3jL+ioQfCu+MiaTAu0pJblA/5gyIz
-fYnKD9On0at5m2QTYNoPyoi+DtlK/AQb+hziEnnsq0g2kG6yfiREB4M4EsbvRYMm
-FjoDVSIipnWr3wvwOmBlo9YEMTTtXHPNR5cGHZn6spBRUXir8NdRlz0CFxsUzd+i
-9whZPnUORyprDZEmFVleNvkvs3kk7sdbNmInlLFdY9bsVx0AM80Bq2KSjuC7kWat
-8d5LLhUIc00p+IRHQPAri9Bb1aX1AVBcAyqhUvahz4qiM8/lrWDepYAeqJeFtHzS
-4NfZHJGxQqK0qycj0WzzRCdzmDjKDTCLfMCU0Bp++tbthD42BlPfr1ifgBZ2y54M
-dKxSEJMyKAA5KCzadRLnaTA427ei4tvw599yvcxvYGoyRVvLzi/eqWD3o8ENKKbe
-l+z8l+3C2ZwYWm1hAn3AVzHb4n1dfuUpEQ82syfuqCcLAFYhPMSIBMsrteeYgddM
-XNtg/VC+tDI=
+bC9nZXQwHQYDVR0OBBYEFPDsMM/q5ErwDwyRX3ZL5W4SNZ4UMA4GA1UdDwEB/wQE
+AwIE8DANBgkqhkiG9w0BAQsFAAOCAgEAh6ujo0JZBb3ys59wsN7SC+uyxZuix7mx
+Uwa0yiC0Dbp6KsTIxJ3UZirgsHkwOXiYU3i/LVZCG7X3YVcRxL6Ej9Ho2OKZzd3Q
+TAdTi262Sm2LDdXTsFy/wmmkVr9v4zJgA6/KxamaroJG6Gvxk9iJs+Zwp1N91iBZ
+K3JnhK7vmiy73qo4TbFxMnYe9ZNOCI6HDArd0b2GxUspjIIeUx3X9OU4VgnK8JBe
+IJX9Fv+ZhhW12bns3LTNBXTrq5Oa7vKChxJtdBCpU73P5bKhr5k4/rHvAmM4Vzo1
++jJHA0g0OZOPRdUcLs8Z5F/6YTD1M41AY9Wnb+dW9XeTcJngmCP5r/1z6USl4vpz
+V0td/ggIF7IRKl6q24GXFstccMj3A7egfnv0BWVbdlQJKF35rg/GtiXJ0BksyJXN
+DxTmxX1RmbvK3KZRocjYlPlW88Z1wbi5MF//wbHESrGBVe2IQ9XlCNKtUhV6nSYx
+IanLtwRe/TsR51jcANW8ZkgpuBMj3wOLNj/nFBM7e0RiEK8LNEKoOIL5ca05bt9b
+CCYpTZ0ggJenmaSYMP58WZB+EOs97a1yn3cCiouFbGusEaG44FJVbQ6A9kzVBgfs
+C9oVfwvign9orWBiIZArLAj5mAeCfa6QWRFumq9nnXkXr1mephnSarA3yjSnnOXi
+3c3pDFm7LcM=
 -----END CERTIFICATE-----"</t>
   </si>
   <si>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
ver 2: commit to date
</commit_message>
<xml_diff>
--- a/DesktopApp/bin/Release/file/ExportExcelCSR.Dialog.xlsx
+++ b/DesktopApp/bin/Release/file/ExportExcelCSR.Dialog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7116"/>
   </bookViews>
   <sheets>
     <sheet name="ToolResult" sheetId="1" r:id="rId1"/>
@@ -19,44 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>STT</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>TelephoneNumber</t>
+  </si>
+  <si>
+    <t>Locality</t>
+  </si>
+  <si>
+    <t>StateProvince</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>CustomerPhoneNumber</t>
+  </si>
+  <si>
+    <t>CustomerEmail</t>
   </si>
   <si>
     <t>CSR</t>
-  </si>
-  <si>
-    <t>Certificate</t>
-  </si>
-  <si>
-    <t>Cert Chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-----BEGIN CERTIFICATE REQUEST-----
-MIICtDCCAZwCAQAwcTEVMBMGA1UEAwwMTmd1eWVuIFZhbiBCMRQwEgYDVQQLDAtD
-b25nIFR5IEFCQzEUMBIGA1UECgwLQ29uZyBUeSBBQkMxCzAJBgNVBAYTAlZOMQ8w
-DQYDVQQHDAZRdWFuIDExDjAMBgNVBAgMBVRQSENNMIIBIjANBgkqhkiG9w0BAQEF
-AAOCAQ8AMIIBCgKCAQEAoVlULf4bVjUPVtl6WxvLWdE2lHGi6t3iTPqIgwMrPM0y
-ag/mz3AQN4njCtyRfHbwb6cIYrmxeNCC9iDqaOcFC1L97s7kH4czXTa5ro4qO34S
-7cKtucQBH+TqRW43gKZknwLCFdnDf07+/ltX9Nsg3u629ZRRKlqn5a8DMUBAqK9s
-ZJYlRek8MAw+XVSJ97JJACXhvmPKHneeb5Ecqtg7Gw7cX4R3lmZc5Gas+g0hShsd
-9YBnNZi7V9GKFA95Om1g3VQUhJLTvd6PWPz3Gltr1mHRU45O2o/MkxnlH0y63zp0
-Gnbb98kr+tsSi1A4gSqWAGX4c6ZUiqk1Boz5bOKSMwIDAQABMA0GCSqGSIb3DQEB
-BQUAA4IBAQA3DPP0Dl2j0kl0yvTriU1Urc0mwsKKWH69nT/C5GyMpba3okHtfqnq
-A6rvuDwWep4XxGcHIx0px8YCxRpAjKzkkIguunniR7/BF9XOzyTBu+vFxsdGCt3C
-1/8gvEA7j73iFSckeB13jEUgFAyMTCvYLlTtS6FsV6BCdl9ecv4W+hEwlcADkqUu
-Ar9CfR+0rdAsrfgeMUYAXeN6tY55azKvfzbSBkcCvh8b7Q6/49Fhr/mFLMiY/x1V
-fstxIX3QDv4qOZPa5wQCW2o/Eyednt2LzAhut5EsvEqko4BlWzFuPThaG052KANJ
-ZDdLD1VmRKdjcCJFYfZGlThwxRv7OKmO
------END CERTIFICATE REQUEST-----
-</t>
-  </si>
-  <si>
-    <t>MIIEFzCCAv+gAwIBAgIQUg2ZAIOhDZYGdNIICqql5jANBgkqhkiG9w0BAQsFADCBozELMAkGA1UEBhMCVk4xMzAxBgNVBAoMKk1pbmlzdHJ5IG9mIEluZm9ybWF0aW9uIGFuZCBDb21tdW5pY2F0aW9uczE8MDoGA1UECwwzTmF0aW9uYWwgQ2VudHJlIG9mIERpZ2l0YWwgU2lnbmF0dXJlIEF1dGhlbnRpY2F0aW9uMSEwHwYDVQQDDBhWaWV0bmFtIE5hdGlvbmFsIFJvb3QgQ0EwHhcNMjExMTA5MDIwMjU2WhcNMjYxMTA4MDIwMjU2WjBAMQswCQYDVQQGEwJWTjEiMCAGA1UECgwZSS1DQSBPTkxJTkUgTUVESUEgVklFVE5BTTENMAsGA1UEAwwESS1DQTCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAKX124bkZ1BkanyJXU1FiwJmCewZorjaHxDt1xey+Nw30xRRgcLL14bSpRNvdIlhGGQVZntLcr5euPdMxm9tyRqPruLBiDepSiAqI8Y2koPiufLLfEYy9BHexLV6L3SarMcVxYs/sxEHzpa5oKoNcOU1zU93b0WSwipXhXZoSJ1wuqcDusHiejfbrTCRMKeO/urd8S+sEx0QOIAvwbLbyNcjiGTWIC/13rNp0Yj6z0ioxLsK7WHon2Q9IcyzTAMhJq9bzO2QxxpZhs+5Gb8z/figloco346UCH3HczAAJ6dBNNiF5parP4EffO2hyNoRKBGF7poT6Lo0PEuRgAOrDn8CAwEAAaOBqDCBpTAPBgNVHRMBAf8EBTADAQH/MB8GA1UdIwQYMBaAFDpCowulPxVK/Rq2Ya+6acwTkQAqMEIGA1UdHwQ7MDkwN6A1oDOGMWh0dHBzOi8vbW9iaWxlLWlkLnZuL2Rvd25sb2FkL3RlbXAvbWljcm9vdDI1Ni5jcmwwHQYDVR0OBBYEFIKuRopmlye2dIqcMBpXhLMyqPziMA4GA1UdDwEB/wQEAwIBhjANBgkqhkiG9w0BAQsFAAOCAQEAQkS3E1sDc3SAl0u39pP+XvH+ZF2pHYYaf+q5F7rs2ejteTqBns0tg0hfxzU4mZM79pCYwQDzx2Sfuzk8lglyKcIvi/ogZElgNe161cd9eANwtQuZlXzI13kZRUafwh0b6StXXX8EkUzbjt4DAuQeL45Uxr5PJVWqw0uIdX5uBYRRBJGFAqxrHx/O0pTwZ6WTRYqvkf+Eq65oB8A9lxd8c1lPPG+uKSPAvNOzJhNfwO7VcjndmorES2Zfq+oKDFEt8RxzoLhJ3aAmwWfYQH9a1XSrdPoIDPL39Fh/rRAIRN6dRslAmEdGdv9/DsMBVsm8gyi+KaJrMYf/mwMkVjORFw==MIIENTCCAx2gAwIBAgIQYwQDvZu4oRy9ebDWcubo0DANBgkqhkiG9w0BAQsFADCBozELMAkGA1UEBhMCVk4xMzAxBgNVBAoMKk1pbmlzdHJ5IG9mIEluZm9ybWF0aW9uIGFuZCBDb21tdW5pY2F0aW9uczE8MDoGA1UECwwzTmF0aW9uYWwgQ2VudHJlIG9mIERpZ2l0YWwgU2lnbmF0dXJlIEF1dGhlbnRpY2F0aW9uMSEwHwYDVQQDDBhWaWV0bmFtIE5hdGlvbmFsIFJvb3QgQ0EwHhcNMjEwNTExMTAzODE2WhcNNDEwNTA2MTAzODE2WjCBozELMAkGA1UEBhMCVk4xMzAxBgNVBAoMKk1pbmlzdHJ5IG9mIEluZm9ybWF0aW9uIGFuZCBDb21tdW5pY2F0aW9uczE8MDoGA1UECwwzTmF0aW9uYWwgQ2VudHJlIG9mIERpZ2l0YWwgU2lnbmF0dXJlIEF1dGhlbnRpY2F0aW9uMSEwHwYDVQQDDBhWaWV0bmFtIE5hdGlvbmFsIFJvb3QgQ0EwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCb6eUiU9eMzQwm412Gk64UXQMC2jAbDNkKHQWTuQOA7Bs5aTcFvTdKyydcL040BTlODP0kljQDLG54A0oeWiWU2Db1sUeAw7zri7Enqfct9wduowIYa8832QF7ZuGm7B+9H957t5KYlO4OL/4sVQCf0QxpPjFxlvNVoIKJPCIolJ8F2cSW1KVRBn2LzkpiG8UkyB0SWKDZM94tdSYpWVAm4+/di15YXTDQbRtLz2L40YrpcWKh5PqNbeDBz8HSSGGIDdJEvtQtlvXMjUqcRPK9izAXjjuOhSxdYSFtvORxcI/kBKqfZivXtuOl1Oj62PXFXg3A/gcclULGhxzHxBojAgMBAAGjYzBhMA8GA1UdEwEB/wQFMAMBAf8wHwYDVR0jBBgwFoAUOkKjC6U/FUr9GrZhr7ppzBORACowHQYDVR0OBBYEFDpCowulPxVK/Rq2Ya+6acwTkQAqMA4GA1UdDwEB/wQEAwIBhjANBgkqhkiG9w0BAQsFAAOCAQEAB+3YVRZWqOjyjSaTP7c6Oplo8jfwf16YV/2PTaDrpJHg/vvBKlQCjv8as2uLffhrecfL92BNzY7c9CRgFFo48JRyoTxYSxgildaaFmjKinv1AX6Xvz6j0dpE0aFynCaxEhsATSYOQMjUG73xdv2gmXG5jk9bu+RjPluVxD5YUkwE76IDqMZXEL7EiMEGSstTrsXKPaN4z6YqiTs59XHYZTJv6btmh5IiUNLG3GHZiNWfVlxeEwhXkFoHrV7nMYuQCh3wFK4/OegIgdREWTQsvKpIC15DzASfyp1SJfU9k4R0DY175IIYfTQ6y6o7bp7j7RYQJwgbmaZ3O4Ex4l6Prw==</t>
-  </si>
-  <si>
-    <t>MIIEsjCCA5qgAwIBAgIQVAEBEks9a87DsocTaO00pzANBgkqhkiG9w0BAQsFADBAMQswCQYDVQQGEwJWTjEiMCAGA1UECgwZSS1DQSBPTkxJTkUgTUVESUEgVklFVE5BTTENMAsGA1UEAwwESS1DQTAeFw0yMjA4MDkwNDQ2MDdaFw0yMzA4MTAwNDQ2MDdaMIGYMQswCQYDVQQGEwJWTjEXMBUGA1UECAwOSOG7kyBDaMOtIE1pbmgxGzAZBgNVBAoMEk5ndXllbiBWYW4gVGVzdCAxMDEVMBMGA1UECwwMQ29uZyBUeSBBQkNEMRswGQYDVQQDDBJOZ3V5ZW4gVmFuIFRlc3QgMTAxHzAdBgoJkiaJk/IsZAEBDA9NU1Q6MTIzNDU2NzgwMTAwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQChWVQt/htWNQ9W2XpbG8tZ0TaUcaLq3eJM+oiDAys8zTJqD+bPcBA3ieMK3JF8dvBvpwhiubF40IL2IOpo5wULUv3uzuQfhzNdNrmujio7fhLtwq25xAEf5OpFbjeApmSfAsIV2cN/Tv7+W1f02yDe7rb1lFEqWqflrwMxQECor2xkliVF6TwwDD5dVIn3skkAJeG+Y8oed55vkRyq2DsbDtxfhHeWZlzkZqz6DSFKGx31gGc1mLtX0YoUD3k6bWDdVBSEktO93o9Y/PcaW2vWYdFTjk7aj8yTGeUfTLrfOnQadtv3ySv62xKLUDiBKpYAZfhzplSKqTUGjPls4pIzAgMBAAGjggFNMIIBSTAMBgNVHRMBAf8EAjAAMB8GA1UdIwQYMBaAFIKuRopmlye2dIqcMBpXhLMyqPziMDkGCCsGAQUFBwEBBC0wKzApBggrBgEFBQcwAYYdaHR0cDovL29jc3AuaS1jYS52bi9yZXNwb25kZXIwTwYDVR0gBEgwRjBEBgsrBgEEAYHtAwEEATA1MDMGCCsGAQUFBwIBFidodHRwOi8vZGljaHZ1ZGllbnR1LmZwdC5jb20udm4vY3BzLmh0bWwwNAYDVR0lBC0wKwYIKwYBBQUHAwIGCCsGAQUFBwMEBgorBgEEAYI3CgMMBgkqhkiG9y8BAQUwJwYDVR0fBCAwHjAcoBqgGIYWaHR0cDovL2ktY2Eudm4vcHViL2NybDAdBgNVHQ4EFgQUTjIjQWAgjq35sFm2Ao24BX74/mowDgYDVR0PAQH/BAQDAgTwMA0GCSqGSIb3DQEBCwUAA4IBAQBEisExAuBDhLuh/cTn2ksRns2wADGyJDADOn9WVmFWIjU0DLCvjKWUVMOOuSKnDHsfLbL2VKyYq8X57DmL1D8Wx9Yyvl6CJWXSZHsusFWZi2x+Uz41bRaDA38eXvKqnRs6x6idGbZYIvZ81wTV7Mo8Zfr+OE+Ae0qc5poskcHUnQQ3cJU6mSy/h8I1CIXn6d4nWdOeiAVxYHqLODDBJyr73g0su37UDB3fjKLG3OSI5e/Vtz+4+yLg7+GL27WW/10X3ebwxxHvfuvYsiUiDKRACwN4mNyaA67HxY6Emt6tT+9+ANVRHdzVRtWOugJeVNcwtqA7En08y7VBtpTnIK/6</t>
   </si>
 </sst>
 </file>
@@ -374,19 +360,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="4" width="46.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="35.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,19 +391,17 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>